<commit_message>
major update, calibration + new trig + FDR + FA
</commit_message>
<xml_diff>
--- a/experiment.xlsx
+++ b/experiment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard Naar\Documents\dok\TARU\EEGManyLabs\Task\spotlight_replication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcadmin\Documents\dok\TARU\PROJEKTID\EEGManyLabs\Task\spotlight_replication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF177771-75FE-4383-AFD6-7DE21709BF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061DF40F-2B63-4A99-A090-69366DFF32B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -369,7 +369,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A11" sqref="A11:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,13 +408,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -422,13 +422,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -436,13 +436,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -450,13 +450,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -478,10 +478,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -506,13 +506,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -520,13 +520,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -548,10 +548,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -561,6 +561,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D13">
+    <sortCondition ref="A1:A13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>